<commit_message>
added data from 6/19 hatchery day
</commit_message>
<xml_diff>
--- a/data/outplanting/transfer_PointWhitney_record.xlsx
+++ b/data/outplanting/transfer_PointWhitney_record.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashuffmyer/MyProjects/oysters/project-gigas-conditioning/data/outplanting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6A49DA6-8197-2048-89BF-601EAF3413E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10FC8CC6-1537-8244-87A2-FD418AF7BA7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3740" yWindow="1300" windowWidth="25800" windowHeight="16940" xr2:uid="{254376F0-C3E5-EB47-AB6A-F0D3E9CC467B}"/>
+    <workbookView xWindow="4440" yWindow="1300" windowWidth="25800" windowHeight="16940" xr2:uid="{254376F0-C3E5-EB47-AB6A-F0D3E9CC467B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>Name/Group</t>
   </si>
@@ -75,6 +75,15 @@
   </si>
   <si>
     <t>Ariana Huffmyer, Steven Roberts; University of Washington</t>
+  </si>
+  <si>
+    <t>Juen 25 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Goose Point Oyster Co. </t>
+  </si>
+  <si>
+    <t>7081 Niawiakum St Hwy #101, Bay Center, WA 98527</t>
   </si>
 </sst>
 </file>
@@ -97,12 +106,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -117,9 +132,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76AF56AC-ECFB-2744-906C-25C6B61D5B11}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -517,6 +533,27 @@
         <v>7</v>
       </c>
     </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added outplant permit record
</commit_message>
<xml_diff>
--- a/data/outplanting/transfer_PointWhitney_record.xlsx
+++ b/data/outplanting/transfer_PointWhitney_record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashuffmyer/MyProjects/oysters/project-gigas-conditioning/data/outplanting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10FC8CC6-1537-8244-87A2-FD418AF7BA7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2941CF49-560A-384E-B59D-786016A317EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4440" yWindow="1300" windowWidth="25800" windowHeight="16940" xr2:uid="{254376F0-C3E5-EB47-AB6A-F0D3E9CC467B}"/>
   </bookViews>
@@ -77,13 +77,13 @@
     <t>Ariana Huffmyer, Steven Roberts; University of Washington</t>
   </si>
   <si>
-    <t>Juen 25 2024</t>
-  </si>
-  <si>
     <t xml:space="preserve">Goose Point Oyster Co. </t>
   </si>
   <si>
     <t>7081 Niawiakum St Hwy #101, Bay Center, WA 98527</t>
+  </si>
+  <si>
+    <t>June 25 2024</t>
   </si>
 </sst>
 </file>
@@ -106,18 +106,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -135,7 +129,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -473,7 +467,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -540,15 +534,17 @@
       <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="2"/>
+      <c r="C3" s="2">
+        <v>1400</v>
+      </c>
       <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>14</v>
-      </c>
-      <c r="F3" t="s">
-        <v>15</v>
       </c>
       <c r="G3" t="s">
         <v>7</v>

</xml_diff>